<commit_message>
Added rate base benchmarks
</commit_message>
<xml_diff>
--- a/Source/DCAF Benchmark.xlsx
+++ b/Source/DCAF Benchmark.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Benjamin\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87C62B0A-E985-4ED0-8782-6FB38BCF2998}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{508D008A-C17F-4F18-AB5C-138AF82A627D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12360" windowHeight="6113" xr2:uid="{D588E70F-352D-4195-AAB7-B3AB4A8838ED}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="50">
   <si>
     <t>Test</t>
   </si>
@@ -141,6 +141,45 @@
   </si>
   <si>
     <t>period</t>
+  </si>
+  <si>
+    <t>100 sv r 10 hz</t>
+  </si>
+  <si>
+    <t>Bench_100_sv_r_10_hz</t>
+  </si>
+  <si>
+    <t>100 sv r 20 hz</t>
+  </si>
+  <si>
+    <t>100 sv r 100 hz</t>
+  </si>
+  <si>
+    <t>100 sv r 200 hz</t>
+  </si>
+  <si>
+    <t>100 sv r 500 hz</t>
+  </si>
+  <si>
+    <t>100 sv r 1000 hz</t>
+  </si>
+  <si>
+    <t>Bench_100_sv_r_20_hz</t>
+  </si>
+  <si>
+    <t>Bench_100_sv_r_100_hz</t>
+  </si>
+  <si>
+    <t>Bench_100_sv_r_200_hz</t>
+  </si>
+  <si>
+    <t>Bench_100_sv_r_500_hz</t>
+  </si>
+  <si>
+    <t>Predicted</t>
+  </si>
+  <si>
+    <t>Aprox Input</t>
   </si>
 </sst>
 </file>
@@ -166,12 +205,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -187,11 +232,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="48" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -507,10 +554,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DC2C9AD-2056-4389-8151-32325A5C9EE8}">
-  <dimension ref="A1:K27"/>
+  <dimension ref="A1:K39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -566,18 +613,18 @@
       <c r="B2">
         <v>0</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="2">
         <v>0</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="3">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="3">
         <v>0</v>
       </c>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
       <c r="J2">
         <v>9030</v>
       </c>
@@ -592,21 +639,21 @@
       <c r="B3">
         <v>0</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="2">
         <v>1000</v>
       </c>
       <c r="D3" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="3">
         <v>4.5999999999999999E-2</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="3">
         <v>2.1000000000000001E-2</v>
       </c>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
       <c r="J3">
         <v>9030</v>
       </c>
@@ -621,25 +668,25 @@
       <c r="B4">
         <v>10</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="2">
         <v>1000</v>
       </c>
       <c r="D4" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="3">
         <v>4.8000000000000001E-2</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="3">
         <v>2.3800000000000002E-2</v>
       </c>
-      <c r="G4" s="1">
+      <c r="G4" s="2">
         <v>6.9999999999999999E-6</v>
       </c>
-      <c r="H4" s="1">
+      <c r="H4" s="2">
         <v>1.9E-6</v>
       </c>
-      <c r="I4" s="1">
+      <c r="I4" s="2">
         <v>6.0000000000000002E-6</v>
       </c>
       <c r="J4">
@@ -656,25 +703,25 @@
       <c r="B5">
         <v>100</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="2">
         <v>1000</v>
       </c>
       <c r="D5" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="3">
         <v>5.2999999999999999E-2</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="3">
         <v>2.8000000000000001E-2</v>
       </c>
-      <c r="G5" s="1">
+      <c r="G5" s="2">
         <v>1.5999999999999999E-5</v>
       </c>
-      <c r="H5" s="1">
+      <c r="H5" s="2">
         <v>1.9999999999999999E-6</v>
       </c>
-      <c r="I5" s="1">
+      <c r="I5" s="2">
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="J5">
@@ -691,25 +738,25 @@
       <c r="B6">
         <v>1000</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="2">
         <v>1000</v>
       </c>
       <c r="D6" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="3">
         <v>0.10299999999999999</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="3">
         <v>7.8E-2</v>
       </c>
-      <c r="G6" s="1">
+      <c r="G6" s="2">
         <v>1.1E-4</v>
       </c>
-      <c r="H6" s="1">
+      <c r="H6" s="2">
         <v>1.9999999999999999E-6</v>
       </c>
-      <c r="I6" s="1">
+      <c r="I6" s="2">
         <v>1.0900000000000001E-5</v>
       </c>
       <c r="J6">
@@ -726,25 +773,25 @@
       <c r="B7">
         <v>10</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="2">
         <v>1000</v>
       </c>
       <c r="D7" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="3">
         <v>0.23799999999999999</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="3">
         <v>0.21</v>
       </c>
-      <c r="G7" s="1">
+      <c r="G7" s="2">
         <v>9.5000000000000001E-7</v>
       </c>
-      <c r="H7" s="1">
+      <c r="H7" s="2">
         <v>3.6999999999999999E-4</v>
       </c>
-      <c r="I7" s="1">
+      <c r="I7" s="2">
         <v>1.5E-5</v>
       </c>
       <c r="J7">
@@ -761,26 +808,26 @@
       <c r="B8">
         <v>100</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="2">
         <v>1000</v>
       </c>
       <c r="D8" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="F8" s="2">
-        <v>0.499</v>
-      </c>
-      <c r="G8" s="1">
+      <c r="E8" s="3">
+        <v>0.38429999999999997</v>
+      </c>
+      <c r="F8" s="3">
+        <v>0.36</v>
+      </c>
+      <c r="G8" s="2">
         <v>8.9999999999999996E-7</v>
       </c>
-      <c r="H8" s="1">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="I8" s="1">
-        <v>2.0000000000000002E-5</v>
+      <c r="H8" s="2">
+        <v>6.6E-4</v>
+      </c>
+      <c r="I8" s="2">
+        <v>1.8499999999999999E-5</v>
       </c>
       <c r="J8">
         <v>9030</v>
@@ -796,7 +843,7 @@
       <c r="B9">
         <v>1000</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="2">
         <v>1000</v>
       </c>
       <c r="D9" t="s">
@@ -816,25 +863,25 @@
       <c r="B10">
         <v>10</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="2">
         <v>1000</v>
       </c>
       <c r="D10" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="3">
         <v>0.245</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F10" s="3">
         <v>0.10099999999999999</v>
       </c>
-      <c r="G10" s="1">
+      <c r="G10" s="2">
         <v>8.9999999999999996E-7</v>
       </c>
-      <c r="H10" s="1">
+      <c r="H10" s="2">
         <v>1.9E-6</v>
       </c>
-      <c r="I10" s="1">
+      <c r="I10" s="2">
         <v>1.3999999999999999E-4</v>
       </c>
       <c r="J10">
@@ -848,25 +895,25 @@
       <c r="B11">
         <v>100</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="2">
         <v>1000</v>
       </c>
       <c r="D11" t="s">
         <v>21</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11" s="3">
         <v>0.52</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F11" s="3">
         <v>0.5</v>
       </c>
-      <c r="G11" s="1">
+      <c r="G11" s="2">
         <v>8.9999999999999996E-7</v>
       </c>
-      <c r="H11" s="1">
+      <c r="H11" s="2">
         <v>1.9E-6</v>
       </c>
-      <c r="I11" s="1">
+      <c r="I11" s="2">
         <v>1.5E-3</v>
       </c>
       <c r="J11">
@@ -880,22 +927,22 @@
       <c r="B12">
         <v>1000</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12" s="2">
         <v>1000</v>
       </c>
       <c r="D12" t="s">
         <v>21</v>
       </c>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
       <c r="J12">
         <v>9030</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>33</v>
       </c>
@@ -908,112 +955,484 @@
       <c r="D19" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A20" s="3">
+      <c r="F19" t="s">
+        <v>49</v>
+      </c>
+      <c r="G19" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A20" s="4">
         <v>1000000</v>
       </c>
       <c r="B20">
         <v>1000</v>
       </c>
-      <c r="C20" s="3">
+      <c r="C20" s="2">
         <f>A20/B20</f>
         <v>1000</v>
       </c>
-      <c r="D20" s="3">
+      <c r="D20" s="2">
         <f>1/C20</f>
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A21" s="3">
+      <c r="F20" s="2">
+        <v>6.9999999999999999E-4</v>
+      </c>
+      <c r="G20" s="1">
+        <f>(F20/D20)/2</f>
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A21" s="4">
         <v>1000000</v>
       </c>
       <c r="B21">
         <v>2000</v>
       </c>
-      <c r="C21" s="3">
+      <c r="C21" s="2">
         <f t="shared" ref="C21:C27" si="0">A21/B21</f>
         <v>500</v>
       </c>
-      <c r="D21" s="3">
+      <c r="D21" s="2">
         <f t="shared" ref="D21:D27" si="1">1/C21</f>
         <v>2E-3</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A22" s="3">
+      <c r="F21" s="2">
+        <v>6.9999999999999999E-4</v>
+      </c>
+      <c r="G21" s="1">
+        <f t="shared" ref="G21:G25" si="2">(F21/D21)/2</f>
+        <v>0.17499999999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A22" s="4">
         <v>1000000</v>
       </c>
       <c r="B22">
         <v>5000</v>
       </c>
-      <c r="C22" s="3">
+      <c r="C22" s="2">
         <f t="shared" si="0"/>
         <v>200</v>
       </c>
-      <c r="D22" s="3">
+      <c r="D22" s="2">
         <f t="shared" si="1"/>
         <v>5.0000000000000001E-3</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A23" s="3">
+      <c r="F22" s="2">
+        <v>6.9999999999999999E-4</v>
+      </c>
+      <c r="G22" s="1">
+        <f t="shared" si="2"/>
+        <v>6.9999999999999993E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A23" s="4">
         <v>1000000</v>
       </c>
       <c r="B23">
         <v>10000</v>
       </c>
-      <c r="C23" s="3">
+      <c r="C23" s="2">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="D23" s="3">
+      <c r="D23" s="2">
         <f t="shared" si="1"/>
         <v>0.01</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A24" s="3">
+      <c r="F23" s="2">
+        <v>6.9999999999999999E-4</v>
+      </c>
+      <c r="G23" s="1">
+        <f t="shared" si="2"/>
+        <v>3.4999999999999996E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A24" s="4">
         <v>1000000</v>
       </c>
       <c r="B24">
         <v>50000</v>
       </c>
-      <c r="C24" s="3">
+      <c r="C24" s="2">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="D24" s="3">
+      <c r="D24" s="2">
         <f t="shared" si="1"/>
         <v>0.05</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A25" s="3">
+      <c r="F24" s="2">
+        <v>6.9999999999999999E-4</v>
+      </c>
+      <c r="G24" s="1">
+        <f t="shared" si="2"/>
+        <v>6.9999999999999993E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A25" s="4">
         <v>1000000</v>
       </c>
       <c r="B25">
         <v>100000</v>
       </c>
-      <c r="C25" s="3">
+      <c r="C25" s="2">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="D25" s="3">
+      <c r="D25" s="2">
         <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A27" s="3"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
+      <c r="F25" s="2">
+        <v>6.9999999999999999E-4</v>
+      </c>
+      <c r="G25" s="1">
+        <f t="shared" si="2"/>
+        <v>3.4999999999999996E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A28" t="s">
+        <v>0</v>
+      </c>
+      <c r="B28" t="s">
+        <v>1</v>
+      </c>
+      <c r="C28" t="s">
+        <v>2</v>
+      </c>
+      <c r="D28" t="s">
+        <v>7</v>
+      </c>
+      <c r="E28" t="s">
+        <v>3</v>
+      </c>
+      <c r="F28" t="s">
+        <v>19</v>
+      </c>
+      <c r="G28" t="s">
+        <v>27</v>
+      </c>
+      <c r="H28" t="s">
+        <v>28</v>
+      </c>
+      <c r="I28" t="s">
+        <v>29</v>
+      </c>
+      <c r="J28" t="s">
+        <v>4</v>
+      </c>
+      <c r="K28" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A29" t="s">
+        <v>6</v>
+      </c>
+      <c r="B29">
+        <v>0</v>
+      </c>
+      <c r="C29" s="2">
+        <v>0</v>
+      </c>
+      <c r="E29" s="3">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="F29" s="3">
+        <v>0</v>
+      </c>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
+      <c r="J29">
+        <v>9030</v>
+      </c>
+      <c r="K29" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A30" t="s">
+        <v>10</v>
+      </c>
+      <c r="B30">
+        <v>0</v>
+      </c>
+      <c r="C30" s="2">
+        <v>1000</v>
+      </c>
+      <c r="D30" t="s">
+        <v>22</v>
+      </c>
+      <c r="E30" s="3">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="F30" s="3">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+      <c r="J30">
+        <v>9030</v>
+      </c>
+      <c r="K30" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A31" t="s">
+        <v>37</v>
+      </c>
+      <c r="B31">
+        <v>100</v>
+      </c>
+      <c r="C31" s="2">
+        <v>10</v>
+      </c>
+      <c r="D31" t="s">
+        <v>21</v>
+      </c>
+      <c r="E31" s="3">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="F31" s="3">
+        <v>1.6999999999999999E-3</v>
+      </c>
+      <c r="G31" s="2">
+        <v>1.9E-6</v>
+      </c>
+      <c r="H31" s="2">
+        <v>7.2999999999999996E-4</v>
+      </c>
+      <c r="I31" s="2">
+        <v>3.0000000000000001E-5</v>
+      </c>
+      <c r="J31">
+        <v>9030</v>
+      </c>
+      <c r="K31" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A32" t="s">
+        <v>39</v>
+      </c>
+      <c r="B32">
+        <v>100</v>
+      </c>
+      <c r="C32" s="2">
+        <v>20</v>
+      </c>
+      <c r="D32" t="s">
+        <v>21</v>
+      </c>
+      <c r="E32" s="3">
+        <v>2.7E-2</v>
+      </c>
+      <c r="F32" s="5">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="G32" s="2">
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="H32" s="2">
+        <v>6.9999999999999999E-4</v>
+      </c>
+      <c r="I32" s="2">
+        <v>2.5000000000000001E-5</v>
+      </c>
+      <c r="J32">
+        <v>9030</v>
+      </c>
+      <c r="K32" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A33" t="s">
+        <v>40</v>
+      </c>
+      <c r="B33">
+        <v>100</v>
+      </c>
+      <c r="C33" s="2">
+        <v>100</v>
+      </c>
+      <c r="D33" t="s">
+        <v>21</v>
+      </c>
+      <c r="E33" s="3">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="F33" s="3">
+        <v>3.7900000000000003E-2</v>
+      </c>
+      <c r="G33" s="2">
+        <v>1.2899999999999999E-6</v>
+      </c>
+      <c r="H33" s="2">
+        <v>6.7000000000000002E-4</v>
+      </c>
+      <c r="I33" s="2">
+        <v>2.5000000000000001E-5</v>
+      </c>
+      <c r="J33">
+        <v>9030</v>
+      </c>
+      <c r="K33" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A34" t="s">
+        <v>41</v>
+      </c>
+      <c r="B34">
+        <v>100</v>
+      </c>
+      <c r="C34" s="2">
+        <v>200</v>
+      </c>
+      <c r="D34" t="s">
+        <v>21</v>
+      </c>
+      <c r="E34" s="3">
+        <v>0.09</v>
+      </c>
+      <c r="F34" s="3">
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="G34" s="2">
+        <v>1.9E-6</v>
+      </c>
+      <c r="H34" s="2">
+        <v>6.8999999999999997E-4</v>
+      </c>
+      <c r="I34" s="4">
+        <v>2.1000000000000001E-4</v>
+      </c>
+      <c r="J34">
+        <v>9030</v>
+      </c>
+      <c r="K34" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A35" t="s">
+        <v>42</v>
+      </c>
+      <c r="B35">
+        <v>100</v>
+      </c>
+      <c r="C35" s="2">
+        <v>500</v>
+      </c>
+      <c r="D35" t="s">
+        <v>21</v>
+      </c>
+      <c r="E35" s="3">
+        <v>0.2056</v>
+      </c>
+      <c r="F35" s="3">
+        <v>0.18</v>
+      </c>
+      <c r="G35" s="2">
+        <v>1.9E-6</v>
+      </c>
+      <c r="H35" s="2">
+        <v>6.7000000000000002E-4</v>
+      </c>
+      <c r="I35" s="2">
+        <v>1.8E-5</v>
+      </c>
+      <c r="J35">
+        <v>9030</v>
+      </c>
+      <c r="K35" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A36" t="s">
+        <v>43</v>
+      </c>
+      <c r="B36">
+        <v>100</v>
+      </c>
+      <c r="C36" s="2">
+        <v>1000</v>
+      </c>
+      <c r="D36" t="s">
+        <v>21</v>
+      </c>
+      <c r="E36" s="3">
+        <v>0.38750000000000001</v>
+      </c>
+      <c r="F36" s="3">
+        <v>0.36</v>
+      </c>
+      <c r="G36" s="2">
+        <v>1.9E-6</v>
+      </c>
+      <c r="H36" s="2">
+        <v>6.7000000000000002E-4</v>
+      </c>
+      <c r="I36" s="2">
+        <v>1.8E-5</v>
+      </c>
+      <c r="J36">
+        <v>9030</v>
+      </c>
+      <c r="K36" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="C37" s="2"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="2"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="C38" s="2"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="2"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="C39" s="2"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
9068 modified scan engine module tests
Adding some rate tests for the 9068 with 32 and 64 variables (1 and 2 9205 modules). These were done using my testing branch of the Scan Engine Module.
</commit_message>
<xml_diff>
--- a/Source/DCAF Benchmark.xlsx
+++ b/Source/DCAF Benchmark.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Benjamin\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\nirvana\se\public\sperez\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{508D008A-C17F-4F18-AB5C-138AF82A627D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{799579C5-E619-4849-AA96-7F4AFFE01564}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12360" windowHeight="6113" xr2:uid="{D588E70F-352D-4195-AAB7-B3AB4A8838ED}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12360" windowHeight="6120" activeTab="1" xr2:uid="{D588E70F-352D-4195-AAB7-B3AB4A8838ED}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="9030_PSP" sheetId="1" r:id="rId1"/>
+    <sheet name="9068_IO" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="59">
   <si>
     <t>Test</t>
   </si>
@@ -180,14 +181,42 @@
   </si>
   <si>
     <t>Aprox Input</t>
+  </si>
+  <si>
+    <t>Purpose</t>
+  </si>
+  <si>
+    <t>Compare the generic PSP module with a modification to use the Scanned Access API</t>
+  </si>
+  <si>
+    <t>Test:</t>
+  </si>
+  <si>
+    <t>1x9205</t>
+  </si>
+  <si>
+    <t>1k</t>
+  </si>
+  <si>
+    <t>2x9206</t>
+  </si>
+  <si>
+    <t>Mod - Scan Engine</t>
+  </si>
+  <si>
+    <t>Note on values:</t>
+  </si>
+  <si>
+    <t>All values are representative snapshots. Not taken through statistical processes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0%"/>
+    <numFmt numFmtId="165" formatCode="0.000000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -232,13 +261,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="48" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -556,22 +586,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DC2C9AD-2056-4389-8151-32325A5C9EE8}">
   <dimension ref="A1:K39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.86328125" customWidth="1"/>
-    <col min="3" max="3" width="10.59765625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.06640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.1328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="14.1328125" customWidth="1"/>
-    <col min="10" max="10" width="5.796875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.85546875" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="14.140625" customWidth="1"/>
+    <col min="10" max="10" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -606,7 +636,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -632,7 +662,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -661,7 +691,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -696,7 +726,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -731,7 +761,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -766,7 +796,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -801,7 +831,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -836,7 +866,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -856,7 +886,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -888,7 +918,7 @@
         <v>9030</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -920,7 +950,7 @@
         <v>9030</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -942,7 +972,7 @@
         <v>9030</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>33</v>
       </c>
@@ -962,7 +992,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>1000000</v>
       </c>
@@ -985,7 +1015,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>1000000</v>
       </c>
@@ -993,11 +1023,11 @@
         <v>2000</v>
       </c>
       <c r="C21" s="2">
-        <f t="shared" ref="C21:C27" si="0">A21/B21</f>
+        <f t="shared" ref="C21:C25" si="0">A21/B21</f>
         <v>500</v>
       </c>
       <c r="D21" s="2">
-        <f t="shared" ref="D21:D27" si="1">1/C21</f>
+        <f t="shared" ref="D21:D25" si="1">1/C21</f>
         <v>2E-3</v>
       </c>
       <c r="F21" s="2">
@@ -1008,7 +1038,7 @@
         <v>0.17499999999999999</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>1000000</v>
       </c>
@@ -1031,7 +1061,7 @@
         <v>6.9999999999999993E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>1000000</v>
       </c>
@@ -1054,7 +1084,7 @@
         <v>3.4999999999999996E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>1000000</v>
       </c>
@@ -1077,7 +1107,7 @@
         <v>6.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>1000000</v>
       </c>
@@ -1100,17 +1130,17 @@
         <v>3.4999999999999996E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>0</v>
       </c>
@@ -1145,7 +1175,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>6</v>
       </c>
@@ -1171,7 +1201,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>10</v>
       </c>
@@ -1200,7 +1230,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>37</v>
       </c>
@@ -1235,7 +1265,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>39</v>
       </c>
@@ -1270,7 +1300,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>40</v>
       </c>
@@ -1305,7 +1335,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>41</v>
       </c>
@@ -1340,7 +1370,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>42</v>
       </c>
@@ -1375,7 +1405,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>43</v>
       </c>
@@ -1410,7 +1440,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C37" s="2"/>
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
@@ -1418,7 +1448,7 @@
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C38" s="2"/>
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
@@ -1426,7 +1456,7 @@
       <c r="H38" s="2"/>
       <c r="I38" s="2"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C39" s="2"/>
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
@@ -1438,4 +1468,180 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{902000FF-913D-4FF4-B991-925C0325E1BE}">
+  <dimension ref="A1:J7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.42578125" customWidth="1"/>
+    <col min="4" max="4" width="19" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" customWidth="1"/>
+    <col min="7" max="7" width="20.5703125" customWidth="1"/>
+    <col min="8" max="8" width="17.85546875" customWidth="1"/>
+    <col min="9" max="9" width="17.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" t="s">
+        <v>29</v>
+      </c>
+      <c r="J3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4">
+        <v>32</v>
+      </c>
+      <c r="C4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4">
+        <v>8.24</v>
+      </c>
+      <c r="F4">
+        <v>3.13</v>
+      </c>
+      <c r="H4">
+        <v>1.8000000000000001E-4</v>
+      </c>
+      <c r="J4">
+        <v>9068</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5">
+        <v>32</v>
+      </c>
+      <c r="C5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D5" t="s">
+        <v>56</v>
+      </c>
+      <c r="E5">
+        <v>7.29</v>
+      </c>
+      <c r="F5">
+        <v>2.2200000000000002</v>
+      </c>
+      <c r="H5" s="6">
+        <v>9.0000000000000006E-5</v>
+      </c>
+      <c r="J5">
+        <v>9068</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B6">
+        <v>64</v>
+      </c>
+      <c r="C6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6">
+        <v>14.85</v>
+      </c>
+      <c r="F6">
+        <v>4.8899999999999997</v>
+      </c>
+      <c r="H6">
+        <v>3.4000000000000002E-4</v>
+      </c>
+      <c r="J6">
+        <v>9068</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B7">
+        <v>64</v>
+      </c>
+      <c r="C7" t="s">
+        <v>54</v>
+      </c>
+      <c r="D7" t="s">
+        <v>56</v>
+      </c>
+      <c r="E7">
+        <v>8.2200000000000006</v>
+      </c>
+      <c r="F7">
+        <v>2.83</v>
+      </c>
+      <c r="H7">
+        <v>1.3999999999999999E-4</v>
+      </c>
+      <c r="J7">
+        <v>9068</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>